<commit_message>
Sheet gen_res in user inputs
</commit_message>
<xml_diff>
--- a/templates/Macro_model.xlsx
+++ b/templates/Macro_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.barla\Documents\Local_codes\HVDCWISE_TEA.jl\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E276B6E1-35ED-4823-A524-7C5555639A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C96294-B1F3-4ABB-A9C5-80D772677895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="8" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
+    <workbookView xWindow="1515" yWindow="4410" windowWidth="15915" windowHeight="8400" activeTab="5" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="8" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="busdc" sheetId="9" r:id="rId3"/>
     <sheet name="load" sheetId="2" r:id="rId4"/>
     <sheet name="gen" sheetId="1" r:id="rId5"/>
-    <sheet name="storage" sheetId="5" r:id="rId6"/>
-    <sheet name="branch" sheetId="3" r:id="rId7"/>
-    <sheet name="branchdc" sheetId="4" r:id="rId8"/>
-    <sheet name="convdc" sheetId="6" r:id="rId9"/>
+    <sheet name="gen_res" sheetId="10" r:id="rId6"/>
+    <sheet name="storage" sheetId="5" r:id="rId7"/>
+    <sheet name="branch" sheetId="3" r:id="rId8"/>
+    <sheet name="branchdc" sheetId="4" r:id="rId9"/>
+    <sheet name="convdc" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="116">
   <si>
     <t>Content</t>
   </si>
@@ -107,9 +108,6 @@
     <t>gen</t>
   </si>
   <si>
-    <t>Generators</t>
-  </si>
-  <si>
     <t>storage</t>
   </si>
   <si>
@@ -194,9 +192,6 @@
     <t>power rating</t>
   </si>
   <si>
-    <t>Wind, Nuclear, Gas, …</t>
-  </si>
-  <si>
     <t>Installed power</t>
   </si>
   <si>
@@ -396,6 +391,30 @@
   </si>
   <si>
     <t>1=monopolar, 2=bipolar</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Wind, PV, …</t>
+  </si>
+  <si>
+    <t>Wind1</t>
+  </si>
+  <si>
+    <t>Nuclear, Gas, …</t>
+  </si>
+  <si>
+    <t>Generators RES</t>
+  </si>
+  <si>
+    <t>Generators non-RES</t>
+  </si>
+  <si>
+    <t>gen_res</t>
+  </si>
+  <si>
+    <t>gen_res id</t>
   </si>
 </sst>
 </file>
@@ -791,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE27698-9DB1-4E7F-9DC7-F345400F49DD}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +887,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDIRECT(A8&amp;"!B1")</f>
@@ -881,14 +900,14 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B15" ca="1" si="0">COUNT(INDIRECT(A9&amp;"!B:B"))</f>
+        <f t="shared" ref="B9:B16" ca="1" si="0">COUNT(INDIRECT(A9&amp;"!B:B"))</f>
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDIRECT(A9&amp;"!B1")</f>
@@ -936,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDIRECT(A11&amp;"!B1")</f>
@@ -957,18 +976,18 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT(A12&amp;"!B1")</f>
-        <v>storage id</v>
+        <v>gen_res id</v>
       </c>
       <c r="E12" t="str" cm="1">
         <f t="array" aca="1" ref="E12" ca="1">INDIRECT(A12&amp;"!C1")</f>
@@ -980,83 +999,71 @@
       </c>
       <c r="G12" t="str" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">INDIRECT(A12&amp;"!E1")</f>
-        <v>production rating</v>
-      </c>
-      <c r="H12" t="str" cm="1">
-        <f t="array" aca="1" ref="H12" ca="1">INDIRECT(A12&amp;"!F1")</f>
-        <v>consumption rating</v>
-      </c>
-      <c r="I12" t="str" cm="1">
-        <f t="array" aca="1" ref="I12" ca="1">INDIRECT(A12&amp;"!G1")</f>
-        <v>initial energy</v>
-      </c>
-      <c r="J12" t="str" cm="1">
-        <f t="array" aca="1" ref="J12" ca="1">INDIRECT(A12&amp;"!H1")</f>
-        <v>energy rating</v>
-      </c>
-      <c r="K12" t="str" cm="1">
-        <f t="array" aca="1" ref="K12" ca="1">INDIRECT(A12&amp;"!I1")</f>
-        <v>production efficiency</v>
-      </c>
-      <c r="L12" t="str" cm="1">
-        <f t="array" aca="1" ref="L12" ca="1">INDIRECT(A12&amp;"!J1")</f>
-        <v>consumption efficiency</v>
+        <v>power rating</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDIRECT(A13&amp;"!B1")</f>
-        <v>branch id</v>
+        <v>storage id</v>
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">INDIRECT(A13&amp;"!C1")</f>
-        <v>from bus id</v>
+        <v>bus id</v>
       </c>
       <c r="F13" t="str" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">INDIRECT(A13&amp;"!D1")</f>
-        <v>to bus id</v>
+        <v>type</v>
       </c>
       <c r="G13" t="str" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">INDIRECT(A13&amp;"!E1")</f>
-        <v>type</v>
+        <v>production rating</v>
       </c>
       <c r="H13" t="str" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">INDIRECT(A13&amp;"!F1")</f>
-        <v>power rating</v>
+        <v>consumption rating</v>
       </c>
       <c r="I13" t="str" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">INDIRECT(A13&amp;"!G1")</f>
-        <v>resistance</v>
+        <v>initial energy</v>
       </c>
       <c r="J13" t="str" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT(A13&amp;"!H1")</f>
-        <v>reactance</v>
+        <v>energy rating</v>
+      </c>
+      <c r="K13" t="str" cm="1">
+        <f t="array" aca="1" ref="K13" ca="1">INDIRECT(A13&amp;"!I1")</f>
+        <v>production efficiency</v>
+      </c>
+      <c r="L13" t="str" cm="1">
+        <f t="array" aca="1" ref="L13" ca="1">INDIRECT(A13&amp;"!J1")</f>
+        <v>consumption efficiency</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">INDIRECT(A14&amp;"!B1")</f>
-        <v>branchdc id</v>
+        <v>branch id</v>
       </c>
       <c r="E14" t="str" cm="1">
         <f t="array" aca="1" ref="E14" ca="1">INDIRECT(A14&amp;"!C1")</f>
@@ -1072,35 +1079,39 @@
       </c>
       <c r="H14" t="str" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">INDIRECT(A14&amp;"!F1")</f>
-        <v>configuration</v>
+        <v>power rating</v>
       </c>
       <c r="I14" t="str" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">INDIRECT(A14&amp;"!G1")</f>
-        <v>power rating</v>
+        <v>resistance</v>
+      </c>
+      <c r="J14" t="str" cm="1">
+        <f t="array" aca="1" ref="J14" ca="1">INDIRECT(A14&amp;"!H1")</f>
+        <v>reactance</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">INDIRECT(A15&amp;"!B1")</f>
-        <v>convdc id</v>
+        <v>branchdc id</v>
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" aca="1" ref="E15" ca="1">INDIRECT(A15&amp;"!C1")</f>
-        <v>AC bus id</v>
+        <v>from bus id</v>
       </c>
       <c r="F15" t="str" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">INDIRECT(A15&amp;"!D1")</f>
-        <v>DC bus id</v>
+        <v>to bus id</v>
       </c>
       <c r="G15" t="str" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">INDIRECT(A15&amp;"!E1")</f>
@@ -1108,6 +1119,42 @@
       </c>
       <c r="H15" t="str" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">INDIRECT(A15&amp;"!F1")</f>
+        <v>configuration</v>
+      </c>
+      <c r="I15" t="str" cm="1">
+        <f t="array" aca="1" ref="I15" ca="1">INDIRECT(A15&amp;"!G1")</f>
+        <v>power rating</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="str" cm="1">
+        <f t="array" aca="1" ref="D16" ca="1">INDIRECT(A16&amp;"!B1")</f>
+        <v>convdc id</v>
+      </c>
+      <c r="E16" t="str" cm="1">
+        <f t="array" aca="1" ref="E16" ca="1">INDIRECT(A16&amp;"!C1")</f>
+        <v>AC bus id</v>
+      </c>
+      <c r="F16" t="str" cm="1">
+        <f t="array" aca="1" ref="F16" ca="1">INDIRECT(A16&amp;"!D1")</f>
+        <v>DC bus id</v>
+      </c>
+      <c r="G16" t="str" cm="1">
+        <f t="array" aca="1" ref="G16" ca="1">INDIRECT(A16&amp;"!E1")</f>
+        <v>type</v>
+      </c>
+      <c r="H16" t="str" cm="1">
+        <f t="array" aca="1" ref="H16" ca="1">INDIRECT(A16&amp;"!F1")</f>
         <v>configuration</v>
       </c>
     </row>
@@ -1116,6 +1163,137 @@
     <mergeCell ref="D7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24A61C9-BE98-4308-A22E-A5F77C928B7D}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1134,24 +1312,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,15 +1337,15 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1178,7 +1356,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1207,24 +1385,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1232,15 +1410,15 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1251,7 +1429,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1281,54 +1459,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1336,30 +1514,30 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1368,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E4">
         <v>15000</v>
@@ -1394,43 +1572,43 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,21 +1616,21 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1461,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E4">
         <v>10000</v>
@@ -1473,6 +1651,89 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47D6FD1-71FC-46C3-A3CF-85733EF09421}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0E26B5-A4C1-4414-BF01-B67D804BCB2D}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -1484,72 +1745,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1557,39 +1818,39 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" t="s">
         <v>54</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>55</v>
       </c>
-      <c r="G3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>56</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>57</v>
-      </c>
-      <c r="J3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1598,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4">
         <v>2000</v>
@@ -1628,7 +1889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE3F783-0E85-4D87-B4F5-59C485B9EADC}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1640,54 +1901,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1695,30 +1956,30 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>69</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1730,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F4">
         <v>1000</v>
@@ -1756,7 +2017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC41CEF-3F39-44ED-97E0-2E32E766EF7A}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1768,54 +2029,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
         <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1823,30 +2084,30 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
         <v>74</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>75</v>
-      </c>
-      <c r="F3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1858,7 +2119,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1883,147 +2144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24A61C9-BE98-4308-A22E-A5F77C928B7D}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
@@ -2033,6 +2154,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2277,20 +2407,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7ED9F52-07AC-4C0A-AC76-FFC7BB308E31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DAE2862-7911-45BF-8962-6BF015BBFC66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
     <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7ED9F52-07AC-4C0A-AC76-FFC7BB308E31}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
No temporary files in matlab_tools folder
</commit_message>
<xml_diff>
--- a/templates/Macro_model.xlsx
+++ b/templates/Macro_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.barla\Documents\Local_codes\HVDCWISE_TEA.jl\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C96294-B1F3-4ABB-A9C5-80D772677895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729428E3-1211-469D-B08F-4AECCD8CBA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="4410" windowWidth="15915" windowHeight="8400" activeTab="5" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="8" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="117">
   <si>
     <t>Content</t>
   </si>
@@ -159,9 +159,6 @@
     <t>All ids must be different.</t>
   </si>
   <si>
-    <t>Nominal voltage expected at this bus. Phase-to-phase voltage if AC, pole-to-ground voltage if DC.</t>
-  </si>
-  <si>
     <t>load id</t>
   </si>
   <si>
@@ -415,6 +412,12 @@
   </si>
   <si>
     <t>gen_res id</t>
+  </si>
+  <si>
+    <t>Nominal voltage (phas-to-phase) expected at this bus.</t>
+  </si>
+  <si>
+    <t>Nominal voltage (pole-to-ground) expected at this bus.</t>
   </si>
 </sst>
 </file>
@@ -816,47 +819,47 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -878,7 +881,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -887,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDIRECT(A8&amp;"!B1")</f>
@@ -898,16 +901,16 @@
         <v>base voltage</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9">
         <f t="shared" ref="B9:B16" ca="1" si="0">COUNT(INDIRECT(A9&amp;"!B:B"))</f>
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDIRECT(A9&amp;"!B1")</f>
@@ -918,7 +921,7 @@
         <v>base voltage</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -946,7 +949,7 @@
         <v>power rating</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -955,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDIRECT(A11&amp;"!B1")</f>
@@ -974,16 +977,16 @@
         <v>power rating</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT(A12&amp;"!B1")</f>
@@ -1002,7 +1005,7 @@
         <v>power rating</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>consumption efficiency</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>reactance</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>power rating</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1174,32 +1177,32 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1219,10 +1222,10 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1230,24 +1233,24 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
         <v>79</v>
       </c>
-      <c r="F3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1259,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1268,9 +1271,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1282,7 +1285,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1302,15 +1305,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1340,12 +1343,12 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1354,9 +1357,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1374,27 +1377,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E426320-1014-411C-AA19-D0D57F06F18F}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1413,12 +1416,12 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1427,9 +1430,9 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1451,18 +1454,18 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>22</v>
@@ -1471,19 +1474,19 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
       <c r="H1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1497,19 +1500,19 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1517,27 +1520,27 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1546,7 +1549,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4">
         <v>15000</v>
@@ -1575,14 +1578,14 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
         <v>22</v>
@@ -1591,10 +1594,10 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1608,10 +1611,10 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1619,18 +1622,18 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1639,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4">
         <v>10000</v>
@@ -1654,18 +1657,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47D6FD1-71FC-46C3-A3CF-85733EF09421}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
         <v>22</v>
@@ -1674,10 +1677,10 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1691,10 +1694,10 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1702,18 +1705,18 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>109</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>110</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1722,7 +1725,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E4">
         <v>10000</v>
@@ -1741,14 +1744,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>22</v>
@@ -1757,28 +1760,28 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1792,28 +1795,28 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
       <c r="I2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
         <v>49</v>
       </c>
-      <c r="J2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1821,36 +1824,36 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" t="s">
-        <v>105</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>54</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>55</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>56</v>
       </c>
-      <c r="K3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1859,7 +1862,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4">
         <v>2000</v>
@@ -1897,35 +1900,35 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1942,16 +1945,16 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1959,27 +1962,27 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>66</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>67</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>68</v>
       </c>
-      <c r="H3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1991,7 +1994,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4">
         <v>1000</v>
@@ -2025,35 +2028,35 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2073,13 +2076,13 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2087,27 +2090,27 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>74</v>
       </c>
-      <c r="H3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2119,7 +2122,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -2145,27 +2148,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
-    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100360305CF8A5F8A4B86568FB88F41EB51" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="7820bdd98b12bbce6701f392baa49827">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xmlns:ns3="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a7208ee71179b2cd86960a83168177e" ns2:_="" ns3:_="">
     <xsd:import namespace="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
@@ -2406,26 +2388,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DAE2862-7911-45BF-8962-6BF015BBFC66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
-    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7ED9F52-07AC-4C0A-AC76-FFC7BB308E31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
+    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51054561-08D6-4033-8FFD-879157D5F173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2442,4 +2426,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7ED9F52-07AC-4C0A-AC76-FFC7BB308E31}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DAE2862-7911-45BF-8962-6BF015BBFC66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
+    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Availablity series coherent for macro-scenarios
</commit_message>
<xml_diff>
--- a/templates/Macro_model.xlsx
+++ b/templates/Macro_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.barla\Documents\Local_codes\HVDCWISE_TEA.jl\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729428E3-1211-469D-B08F-4AECCD8CBA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DA4295-BCA1-4277-8956-16EFB987E229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" firstSheet="4" activeTab="8" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="8" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="121">
   <si>
     <t>Content</t>
   </si>
@@ -285,9 +285,6 @@
     <t>Must be a DC bus defined in the bus tab and different from the from bus. From and to bs voltages must be the same.</t>
   </si>
   <si>
-    <t>DC cable reference</t>
-  </si>
-  <si>
     <t>If MW: maximum power allowed in the DC link. If kA: ampacity (per pole).</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t>DC bus id</t>
   </si>
   <si>
-    <t>Converter reference (ex: MMC 500 MW)</t>
-  </si>
-  <si>
     <t>Maximum power allowed in the converter</t>
   </si>
   <si>
@@ -342,24 +336,12 @@
     <t>AC line 20 km</t>
   </si>
   <si>
-    <t>DC line 20 km</t>
-  </si>
-  <si>
     <t>Conv1</t>
   </si>
   <si>
     <t>Conv2</t>
   </si>
   <si>
-    <t>MMC_1GW</t>
-  </si>
-  <si>
-    <t>OHL_Al_400kV_2x500mm2</t>
-  </si>
-  <si>
-    <t>Cable_Cu_320kV_800mm2</t>
-  </si>
-  <si>
     <t>AC buses</t>
   </si>
   <si>
@@ -418,6 +400,36 @@
   </si>
   <si>
     <t>Nominal voltage (pole-to-ground) expected at this bus.</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>DC cable or DC OHL</t>
+  </si>
+  <si>
+    <t>DC cable</t>
+  </si>
+  <si>
+    <t>Length of th DC branch</t>
+  </si>
+  <si>
+    <t>DC cable 20 km</t>
+  </si>
+  <si>
+    <t>Length of th AC branch (0 if transformer)</t>
+  </si>
+  <si>
+    <t>AC OHL</t>
+  </si>
+  <si>
+    <t>MMC</t>
+  </si>
+  <si>
+    <t>Converter type (not used)</t>
   </si>
 </sst>
 </file>
@@ -819,47 +831,47 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -881,7 +893,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -890,7 +902,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDIRECT(A8&amp;"!B1")</f>
@@ -901,16 +913,16 @@
         <v>base voltage</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B9">
         <f t="shared" ref="B9:B16" ca="1" si="0">COUNT(INDIRECT(A9&amp;"!B:B"))</f>
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDIRECT(A9&amp;"!B1")</f>
@@ -921,7 +933,7 @@
         <v>base voltage</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -949,7 +961,7 @@
         <v>power rating</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -958,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDIRECT(A11&amp;"!B1")</f>
@@ -977,16 +989,16 @@
         <v>power rating</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT(A12&amp;"!B1")</f>
@@ -1005,7 +1017,7 @@
         <v>power rating</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1053,7 +1065,7 @@
         <v>consumption efficiency</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1082,18 +1094,18 @@
       </c>
       <c r="H14" t="str" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">INDIRECT(A14&amp;"!F1")</f>
-        <v>power rating</v>
+        <v>length</v>
       </c>
       <c r="I14" t="str" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">INDIRECT(A14&amp;"!G1")</f>
-        <v>resistance</v>
+        <v>power rating</v>
       </c>
       <c r="J14" t="str" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT(A14&amp;"!H1")</f>
-        <v>reactance</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>resistance</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1122,14 +1134,14 @@
       </c>
       <c r="H15" t="str" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">INDIRECT(A15&amp;"!F1")</f>
-        <v>configuration</v>
+        <v>length</v>
       </c>
       <c r="I15" t="str" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">INDIRECT(A15&amp;"!G1")</f>
-        <v>power rating</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+        <v>configuration</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1174,35 +1186,35 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1225,7 +1237,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1239,18 +1251,18 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1262,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1271,9 +1283,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1285,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1308,12 +1320,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1335,7 +1347,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1343,12 +1355,12 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1357,9 +1369,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1377,27 +1389,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E426320-1014-411C-AA19-D0D57F06F18F}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1408,7 +1420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1416,12 +1428,12 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1430,9 +1442,9 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1454,13 +1466,13 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1483,10 +1495,10 @@
         <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1512,7 +1524,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1529,18 +1541,18 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1549,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4">
         <v>15000</v>
@@ -1578,9 +1590,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1597,7 +1609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1614,7 +1626,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1625,15 +1637,15 @@
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1642,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4">
         <v>10000</v>
@@ -1661,14 +1673,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
         <v>22</v>
@@ -1680,7 +1692,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1708,15 +1720,15 @@
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1725,7 +1737,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E4">
         <v>10000</v>
@@ -1744,9 +1756,9 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1766,7 +1778,7 @@
         <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
         <v>44</v>
@@ -1781,7 +1793,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1816,7 +1828,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1836,7 +1848,7 @@
         <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H3" t="s">
         <v>53</v>
@@ -1851,9 +1863,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1862,7 +1874,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E4">
         <v>2000</v>
@@ -1894,15 +1906,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE3F783-0E85-4D87-B4F5-59C485B9EADC}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1919,16 +1931,19 @@
         <v>23</v>
       </c>
       <c r="F1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>60</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1945,16 +1960,19 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
       </c>
       <c r="H2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1971,18 +1989,21 @@
         <v>65</v>
       </c>
       <c r="F3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" t="s">
         <v>66</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>67</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1994,25 +2015,31 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
         <v>1000</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.03</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{7570D59E-4D6E-4042-B9C5-F369EB8B7077}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{7570D59E-4D6E-4042-B9C5-F369EB8B7077}">
       <formula1>"MW,kA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H2" xr:uid="{6CCDCAFB-D193-4BB4-944B-B96DD26BB55D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I2" xr:uid="{6CCDCAFB-D193-4BB4-944B-B96DD26BB55D}">
       <formula1>"Ohm,pu"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{F1C5D8A5-C885-4ABA-8254-913047A7D20C}">
+      <formula1>"AC OHL,Transformer"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2022,15 +2049,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC41CEF-3F39-44ED-97E0-2E32E766EF7A}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -2047,16 +2074,19 @@
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2073,16 +2103,19 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2096,21 +2129,24 @@
         <v>71</v>
       </c>
       <c r="E3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
         <v>72</v>
       </c>
-      <c r="F3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>73</v>
       </c>
-      <c r="H3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2122,25 +2158,31 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1000</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.03</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{F4C4D698-077A-4FD4-8E3B-93A2469DAA72}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{F4C4D698-077A-4FD4-8E3B-93A2469DAA72}">
       <formula1>"MW,kA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{D28FA82A-5062-475B-8FE8-8D9740D8C9C0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{D28FA82A-5062-475B-8FE8-8D9740D8C9C0}">
       <formula1>"Ohm,pu"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{30F54288-D634-44C3-A062-10557F0B633A}">
+      <formula1>"DC cable,DC OHL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2148,6 +2190,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
+    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100360305CF8A5F8A4B86568FB88F41EB51" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="7820bdd98b12bbce6701f392baa49827">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xmlns:ns3="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a7208ee71179b2cd86960a83168177e" ns2:_="" ns3:_="">
     <xsd:import namespace="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
@@ -2388,7 +2442,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2397,19 +2451,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
-    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DAE2862-7911-45BF-8962-6BF015BBFC66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
+    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51054561-08D6-4033-8FFD-879157D5F173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2428,21 +2481,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7ED9F52-07AC-4C0A-AC76-FFC7BB308E31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DAE2862-7911-45BF-8962-6BF015BBFC66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
-    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enable aggregated lines in AC branches
</commit_message>
<xml_diff>
--- a/templates/Macro_model.xlsx
+++ b/templates/Macro_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.barla\Documents\Local_codes\HVDCWISE_TEA.jl\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DA4295-BCA1-4277-8956-16EFB987E229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3D8339-A4FA-45F8-9AB6-A7A2C37F991F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" firstSheet="4" activeTab="8" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="8" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="123">
   <si>
     <t>Content</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>Converter type (not used)</t>
+  </si>
+  <si>
+    <t>number of lines</t>
+  </si>
+  <si>
+    <t>Number of real lines in parallel. 1 if not a reduced edge</t>
   </si>
 </sst>
 </file>
@@ -827,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE27698-9DB1-4E7F-9DC7-F345400F49DD}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1906,15 +1912,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE3F783-0E85-4D87-B4F5-59C485B9EADC}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1942,8 +1948,11 @@
       <c r="I1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1971,8 +1980,11 @@
       <c r="I2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2000,8 +2012,11 @@
       <c r="I3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -2028,6 +2043,9 @@
       </c>
       <c r="I4">
         <v>0.3</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2051,8 +2069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC41CEF-3F39-44ED-97E0-2E32E766EF7A}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>